<commit_message>
CopyRightObject, AddObject function -pb
</commit_message>
<xml_diff>
--- a/Misc/ghBanners.xlsx
+++ b/Misc/ghBanners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbrower/projects/just-VBA/Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3012C67-CFB8-B945-8321-2281B0904819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3453C37D-62F0-B04B-A5A4-DD8E8DB0737F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11080" yWindow="1000" windowWidth="31900" windowHeight="25740" xr2:uid="{A0BCE7D4-6CEF-2741-A7CB-45C3BE44EC3D}"/>
   </bookViews>
@@ -1350,7 +1350,7 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="462034" y="5714916"/>
+              <a:off x="462034" y="5706158"/>
               <a:ext cx="187734" cy="297273"/>
             </a:xfrm>
             <a:prstGeom prst="rect">

</xml_diff>

<commit_message>
added copylistcol demo -pb
</commit_message>
<xml_diff>
--- a/Misc/ghBanners.xlsx
+++ b/Misc/ghBanners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbrower/projects/just-VBA/Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3453C37D-62F0-B04B-A5A4-DD8E8DB0737F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED69EAF4-2F73-AC44-86C4-D32749D3AB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11080" yWindow="1000" windowWidth="31900" windowHeight="25740" xr2:uid="{A0BCE7D4-6CEF-2741-A7CB-45C3BE44EC3D}"/>
   </bookViews>
@@ -35,14 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t xml:space="preserve">schedule in rhe 8AM to noon timeframe </t>
-  </si>
-  <si>
-    <t>Kristin</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2066,6 +2059,57 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>503621</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30655</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>784762</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>73787</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Reddit -- ITFuture"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02397018-2C1F-2649-950A-3F5C387B8D32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="503621" y="4059621"/>
+          <a:ext cx="281141" cy="446028"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2367,25 +2411,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12AD1E2-8854-9E45-9937-970324FAD2E6}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B26:B27"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="290" zoomScaleNormal="290" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="290" zoomScaleNormal="290" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>